<commit_message>
Update for fall 2022
</commit_message>
<xml_diff>
--- a/Output/Tables_for_paper.xlsx
+++ b/Output/Tables_for_paper.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon.Richar\Work\Projects\Length_weight\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon.Richar\Work\GitRepos\LengthWeight\EBSCrabLengthWeight\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="7170" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="7170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tbl1 Sampling effort" sheetId="1" r:id="rId1"/>
-    <sheet name="Tbl2 ModelParams" sheetId="2" r:id="rId2"/>
-    <sheet name="Tbl3 ANCOVA" sheetId="3" r:id="rId3"/>
-    <sheet name="Tbl4 PctDif" sheetId="4" r:id="rId4"/>
+    <sheet name="Table1a Female and SMBKC_Effort" sheetId="6" r:id="rId2"/>
+    <sheet name="Tbl2 ModelParams" sheetId="2" r:id="rId3"/>
+    <sheet name="Tbl3 ANCOVA" sheetId="3" r:id="rId4"/>
+    <sheet name="Tbl4 PctDif" sheetId="4" r:id="rId5"/>
+    <sheet name="Tbl5Params" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>Year</t>
   </si>
@@ -359,7 +361,106 @@
     <t>EBS CB - Standard</t>
   </si>
   <si>
-    <t>EBS CO Standard</t>
+    <t>BairdiStandard</t>
+  </si>
+  <si>
+    <t>BairdiNewModel</t>
+  </si>
+  <si>
+    <t>BairdiBiasCorrected</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>OpilioStandard</t>
+  </si>
+  <si>
+    <t>OpilioNewModel</t>
+  </si>
+  <si>
+    <t>OpilioBiasCorrected</t>
+  </si>
+  <si>
+    <t>BBRKCStandard</t>
+  </si>
+  <si>
+    <t>BBRKCNewModel</t>
+  </si>
+  <si>
+    <t>BBRKCBiasCorrected</t>
+  </si>
+  <si>
+    <t>NS_Param_a</t>
+  </si>
+  <si>
+    <t>NS_Param_b</t>
+  </si>
+  <si>
+    <t>OS_Param_a</t>
+  </si>
+  <si>
+    <t>OS_Param_b</t>
+  </si>
+  <si>
+    <t>SMBKC - NS</t>
+  </si>
+  <si>
+    <t>SMBKC - OS</t>
+  </si>
+  <si>
+    <t>SMBKC - Standard</t>
+  </si>
+  <si>
+    <t>EBS CB - Matfem - Standard</t>
+  </si>
+  <si>
+    <t>EBS CB - Matfem - NS</t>
+  </si>
+  <si>
+    <t>EBS CB - Matfem - OS</t>
+  </si>
+  <si>
+    <t>EBS CO - Matfem - Standard</t>
+  </si>
+  <si>
+    <t>EBS CO - Standard</t>
+  </si>
+  <si>
+    <t>EBS CO - Matfem - NS</t>
+  </si>
+  <si>
+    <t>EBS CO - Matfem - OS</t>
+  </si>
+  <si>
+    <t>SMBKC - New shell/Old shell</t>
+  </si>
+  <si>
+    <t>p = 0.203</t>
+  </si>
+  <si>
+    <t>EBS CB - Matfem - New shell/Old shell</t>
+  </si>
+  <si>
+    <t>EBS CO - Matfem - New shell/Old shell</t>
+  </si>
+  <si>
+    <t>p = 0.0145</t>
+  </si>
+  <si>
+    <t>p = 0.01452</t>
+  </si>
+  <si>
+    <t>p = 0.0375</t>
+  </si>
+  <si>
+    <t>p = 0.03748</t>
+  </si>
+  <si>
+    <t>p = 3.28e-05</t>
+  </si>
+  <si>
+    <t>p = 3.279e-05</t>
   </si>
 </sst>
 </file>
@@ -369,7 +470,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +488,25 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -411,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -424,18 +544,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,7 +850,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A22" sqref="A22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1198,10 +1329,425 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2001</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2006</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>231</v>
+      </c>
+      <c r="G4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2007</v>
+      </c>
+      <c r="B5">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>158</v>
+      </c>
+      <c r="G5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2008</v>
+      </c>
+      <c r="B6">
+        <v>62</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>84</v>
+      </c>
+      <c r="F6">
+        <v>212</v>
+      </c>
+      <c r="G6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2009</v>
+      </c>
+      <c r="B7">
+        <v>116</v>
+      </c>
+      <c r="C7">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>44</v>
+      </c>
+      <c r="F7">
+        <v>104</v>
+      </c>
+      <c r="G7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2010</v>
+      </c>
+      <c r="B8">
+        <v>267</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>58</v>
+      </c>
+      <c r="E8">
+        <v>140</v>
+      </c>
+      <c r="F8">
+        <v>441</v>
+      </c>
+      <c r="G8">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2011</v>
+      </c>
+      <c r="B9">
+        <v>119</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <v>339</v>
+      </c>
+      <c r="G9">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2012</v>
+      </c>
+      <c r="B10">
+        <v>113</v>
+      </c>
+      <c r="C10">
+        <v>73</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2013</v>
+      </c>
+      <c r="B11">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>657</v>
+      </c>
+      <c r="G11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>74</v>
+      </c>
+      <c r="C12">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>48</v>
+      </c>
+      <c r="E12">
+        <v>217</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2015</v>
+      </c>
+      <c r="B13">
+        <v>54</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>432</v>
+      </c>
+      <c r="G13">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2016</v>
+      </c>
+      <c r="B14">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2017</v>
+      </c>
+      <c r="B15">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>546</v>
+      </c>
+      <c r="G15">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2018</v>
+      </c>
+      <c r="B16">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>93</v>
+      </c>
+      <c r="E16">
+        <v>111</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2019</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>354</v>
+      </c>
+      <c r="G17">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1209,7 +1755,7 @@
     <col min="1" max="1" width="28.6328125" customWidth="1"/>
     <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1222,10 +1768,10 @@
       <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1240,10 +1786,10 @@
       <c r="C2" s="4">
         <v>3.1413340000000001</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="6">
         <v>4.0299999999999998E-4</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="6">
         <v>3.1413340000000001</v>
       </c>
     </row>
@@ -1251,17 +1797,17 @@
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>-7.8496199999999998</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>3.1478860000000002</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <f>EXP(B3)</f>
         <v>3.8990010214434766E-4</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <f>C3</f>
         <v>3.1478860000000002</v>
       </c>
@@ -1270,17 +1816,17 @@
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>-7.6398400000000004</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>3.11117</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <f t="shared" ref="D4:D18" si="0">EXP(B4)</f>
         <v>4.8090539076564213E-4</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <f t="shared" ref="E4:E18" si="1">C4</f>
         <v>3.11117</v>
       </c>
@@ -1289,17 +1835,17 @@
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>-7.5879690000000002</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>3.0992769999999998</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
         <v>5.0650872923577975E-4</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <f t="shared" si="1"/>
         <v>3.0992769999999998</v>
       </c>
@@ -1308,17 +1854,17 @@
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>-7.9068019999999999</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>3.1575449999999998</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
         <v>3.6823030011733082E-4</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <f t="shared" si="1"/>
         <v>3.1575449999999998</v>
       </c>
@@ -1327,16 +1873,16 @@
       <c r="A7" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>-7.8326409999999997</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <v>3.1444019999999999</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>3.9657670000000001E-4</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>3.1444019999999999</v>
       </c>
     </row>
@@ -1344,16 +1890,16 @@
       <c r="A8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>-7.0620799999999999</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>2.9895700000000001</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>8.5699370000000003E-4</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>2.9895700000000001</v>
       </c>
     </row>
@@ -1361,16 +1907,16 @@
       <c r="A9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>-7.72281</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>3.1276600000000001</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>4.4261510000000002E-4</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>3.1276600000000001</v>
       </c>
     </row>
@@ -1378,17 +1924,17 @@
       <c r="A10" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <f>LN(D10)</f>
         <v>-8.2170885989658995</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>3.0221339999999999</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>2.7E-4</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>3.0221339999999999</v>
       </c>
     </row>
@@ -1396,17 +1942,17 @@
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>-8.2045709999999996</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>3.0142540000000002</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <f t="shared" si="0"/>
         <v>2.7340099344839281E-4</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <f t="shared" si="1"/>
         <v>3.0142540000000002</v>
       </c>
@@ -1415,17 +1961,17 @@
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>-8.4782060000000001</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>3.0919660000000002</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <f t="shared" si="0"/>
         <v>2.0795143314962319E-4</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <f t="shared" si="1"/>
         <v>3.0919660000000002</v>
       </c>
@@ -1434,16 +1980,16 @@
       <c r="A13" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>-8.3600499999999993</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>3.0488499999999998</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <v>2.340326E-4</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>3.0488499999999998</v>
       </c>
     </row>
@@ -1451,16 +1997,16 @@
       <c r="A14" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>-9.0331700000000001</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>3.1923499999999998</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <v>1.1938340000000001E-4</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>3.1923499999999998</v>
       </c>
     </row>
@@ -1468,34 +2014,34 @@
       <c r="A15" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>-8.3534299999999995</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>3.0663399999999998</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>2.355871E-4</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>3.0576300000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="9">
+        <v>131</v>
+      </c>
+      <c r="B16" s="7">
         <f>LN(D16)</f>
         <v>-8.2282618995640249</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>3.0972529999999998</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="7">
         <v>2.6699999999999998E-4</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>3.0972529999999998</v>
       </c>
     </row>
@@ -1503,17 +2049,17 @@
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>-8.3476339999999993</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>3.1195089999999999</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <f t="shared" si="0"/>
         <v>2.3695649478204216E-4</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <f t="shared" si="1"/>
         <v>3.1195089999999999</v>
       </c>
@@ -1522,17 +2068,17 @@
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>-7.9782780000000004</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>3.0517479999999999</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <f t="shared" si="0"/>
         <v>3.4282926651053587E-4</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <f t="shared" si="1"/>
         <v>3.0517479999999999</v>
       </c>
@@ -1541,16 +2087,16 @@
       <c r="A19" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>-8.4144070000000006</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="6">
         <v>3.1348600000000002</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="6">
         <v>2.340326E-4</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="6">
         <v>3.1348600000000002</v>
       </c>
     </row>
@@ -1558,16 +2104,16 @@
       <c r="A20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>-8.5887170000000008</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="6">
         <v>3.1736499999999999</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
         <v>1.8619479999999999E-4</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>3.1736499999999999</v>
       </c>
     </row>
@@ -1575,17 +2121,173 @@
       <c r="A21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>-7.9945310000000003</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="6">
         <v>3.0553520000000001</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="6">
         <v>3.3730259999999998E-4</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="6">
         <v>3.0553520000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="7">
+        <f>LN(D26)</f>
+        <v>-7.5969104382725448</v>
+      </c>
+      <c r="C26" s="7">
+        <v>3.1071580000000001</v>
+      </c>
+      <c r="D26" s="7">
+        <v>5.0199999999999995E-4</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3.1071580000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="7">
+        <v>-7.9725450000000002</v>
+      </c>
+      <c r="C27" s="7">
+        <v>3.1765590000000001</v>
+      </c>
+      <c r="D27" s="7">
+        <v>3.4600000000000001E-4</v>
+      </c>
+      <c r="E27" s="7">
+        <v>3.1765590000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="7">
+        <v>-7.5045000000000002</v>
+      </c>
+      <c r="C28" s="7">
+        <v>3.093953</v>
+      </c>
+      <c r="D28" s="7">
+        <v>5.5199999999999997E-4</v>
+      </c>
+      <c r="E28" s="7">
+        <v>3.093953</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="12">
+        <f>LN(D29)</f>
+        <v>-7.7264656825174285</v>
+      </c>
+      <c r="C29" s="12">
+        <v>2.8986860000000001</v>
+      </c>
+      <c r="D29" s="13">
+        <v>4.4099999999999999E-4</v>
+      </c>
+      <c r="E29" s="13">
+        <v>2.8986860000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="12">
+        <v>-7.6935099999999998</v>
+      </c>
+      <c r="C30" s="12">
+        <v>2.88374</v>
+      </c>
+      <c r="D30" s="13">
+        <v>4.5600000000000003E-4</v>
+      </c>
+      <c r="E30" s="13">
+        <v>2.88374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="12">
+        <v>-7.3675620000000004</v>
+      </c>
+      <c r="C31" s="12">
+        <v>2.8240720000000001</v>
+      </c>
+      <c r="D31" s="13">
+        <v>6.3199999999999997E-4</v>
+      </c>
+      <c r="E31" s="13">
+        <v>2.8240720000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="12">
+        <f>LN(D32)</f>
+        <v>-6.7610608998313335</v>
+      </c>
+      <c r="C32" s="12">
+        <v>2.708793</v>
+      </c>
+      <c r="D32" s="13">
+        <v>1.158E-3</v>
+      </c>
+      <c r="E32" s="13">
+        <v>2.708793</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="12">
+        <v>-7.1463679999999998</v>
+      </c>
+      <c r="C33" s="12">
+        <v>2.7990469999999998</v>
+      </c>
+      <c r="D33" s="13">
+        <v>7.8899999999999999E-4</v>
+      </c>
+      <c r="E33" s="13">
+        <v>2.7990469999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="12">
+        <v>-7.381869</v>
+      </c>
+      <c r="C34" s="12">
+        <v>2.8658610000000002</v>
+      </c>
+      <c r="D34" s="13">
+        <v>6.2299999999999996E-4</v>
+      </c>
+      <c r="E34" s="13">
+        <v>2.8658610000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1594,12 +2296,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1745,17 +2449,17 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="I7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="2">
-        <v>0.20300000000000001</v>
+      <c r="J7" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>47</v>
@@ -1819,9 +2523,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
@@ -1895,9 +2599,9 @@
       </c>
     </row>
     <row r="18" spans="9:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="I18" s="6"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="9:12" ht="15.5" x14ac:dyDescent="0.35">
@@ -1975,6 +2679,48 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="9:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I25" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="9:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I26" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="9:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I27" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1987,7 +2733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2016,10 +2762,10 @@
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>0.8159769</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="9">
         <v>0.90791219999999995</v>
       </c>
     </row>
@@ -2027,10 +2773,10 @@
       <c r="A3" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>3.0103610000000001</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>3.1927189999999999</v>
       </c>
     </row>
@@ -2038,10 +2784,10 @@
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>2.3749410000000002</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>2.6935699999999998</v>
       </c>
     </row>
@@ -2049,10 +2795,10 @@
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>1.242149E-2</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>-0.1781421</v>
       </c>
     </row>
@@ -2060,6 +2806,161 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3">
+        <v>2.7340099999999999E-4</v>
+      </c>
+      <c r="C3">
+        <v>3.0142540000000002</v>
+      </c>
+      <c r="D3">
+        <v>2.079514E-4</v>
+      </c>
+      <c r="E3">
+        <v>3.0919660000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4">
+        <v>2.7439860000000001E-4</v>
+      </c>
+      <c r="C4">
+        <v>3.0142540000000002</v>
+      </c>
+      <c r="D4">
+        <v>2.0835839999999999E-4</v>
+      </c>
+      <c r="E4">
+        <v>3.0919660000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6">
+        <v>2.3695650000000001E-4</v>
+      </c>
+      <c r="C6">
+        <v>3.11951</v>
+      </c>
+      <c r="D6">
+        <v>3.428293E-4</v>
+      </c>
+      <c r="E6">
+        <v>3.0517479999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7">
+        <v>2.3778819999999999E-4</v>
+      </c>
+      <c r="C7">
+        <v>3.1195089999999999</v>
+      </c>
+      <c r="D7">
+        <v>3.4347739999999999E-4</v>
+      </c>
+      <c r="E7">
+        <v>3.0517479999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9">
+        <v>3.8990010000000002E-4</v>
+      </c>
+      <c r="C9">
+        <v>3.1478860000000002</v>
+      </c>
+      <c r="D9">
+        <v>4.8090300000000003E-4</v>
+      </c>
+      <c r="E9">
+        <v>3.1111659999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10">
+        <v>3.9084450000000001E-4</v>
+      </c>
+      <c r="C10">
+        <v>3.1478860000000002</v>
+      </c>
+      <c r="D10">
+        <v>4.8189169999999999E-4</v>
+      </c>
+      <c r="E10" s="10">
+        <v>3.1111659999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>